<commit_message>
8 August 2017 barkha
</commit_message>
<xml_diff>
--- a/TestData/LanguagesTestData.xlsx
+++ b/TestData/LanguagesTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>TC_ID</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>AmentitiesList_Title</t>
+  </si>
+  <si>
+    <t>Message_Text1</t>
+  </si>
+  <si>
+    <t>-  Amenidade/serviço</t>
+  </si>
+  <si>
+    <t>Message_Text2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> salvo com sucesso.</t>
   </si>
 </sst>
 </file>
@@ -490,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,7 +513,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,10 +522,10 @@
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
@@ -600,6 +612,18 @@
       </c>
       <c r="D3" t="s">
         <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
9 August 3rd Commit
</commit_message>
<xml_diff>
--- a/TestData/LanguagesTestData.xlsx
+++ b/TestData/LanguagesTestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11340"/>
   </bookViews>
   <sheets>
-    <sheet name="Portuguese" sheetId="1" r:id="rId1"/>
+    <sheet name="Admin_SZ_Portuguese" sheetId="1" r:id="rId1"/>
     <sheet name="Spanish" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>TC_ID</t>
   </si>
@@ -109,13 +109,28 @@
     <t>Message_Text1</t>
   </si>
   <si>
-    <t>-  Amenidade/serviço</t>
-  </si>
-  <si>
     <t>Message_Text2</t>
   </si>
   <si>
     <t xml:space="preserve"> salvo com sucesso.</t>
+  </si>
+  <si>
+    <t>fn_verifyAdditionOfRoom</t>
+  </si>
+  <si>
+    <t>RoomsList_Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> salvo com sucesso</t>
+  </si>
+  <si>
+    <t>Lista de quartos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Quarto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Amenidade/serviço </t>
   </si>
 </sst>
 </file>
@@ -502,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,13 +632,36 @@
         <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
18 August Barkha Commit
</commit_message>
<xml_diff>
--- a/TestData/LanguagesTestData.xlsx
+++ b/TestData/LanguagesTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
   <si>
     <t>TC_ID</t>
   </si>
@@ -143,6 +143,51 @@
   </si>
   <si>
     <t>Lista de taxas dos quartos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> salva com sucesso</t>
+  </si>
+  <si>
+    <t>Status_src</t>
+  </si>
+  <si>
+    <t>on.GIF</t>
+  </si>
+  <si>
+    <t>RoomTypesList_Title</t>
+  </si>
+  <si>
+    <t>Message_Text3</t>
+  </si>
+  <si>
+    <t>Message_Text4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Taxa de quarto </t>
+  </si>
+  <si>
+    <t>Lista de tipos de quarto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tipo de quarto (s) </t>
+  </si>
+  <si>
+    <t>fn_verifyAdditionOfAddOns</t>
+  </si>
+  <si>
+    <t>AddOnsList_Title</t>
+  </si>
+  <si>
+    <t>Lista de adições</t>
+  </si>
+  <si>
+    <t>fn_verifyAddAPackageWithInclusion</t>
+  </si>
+  <si>
+    <t>AddInclusion_Title</t>
+  </si>
+  <si>
+    <t>Adicionar inclusões</t>
   </si>
 </sst>
 </file>
@@ -529,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +600,12 @@
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -702,6 +749,76 @@
       </c>
       <c r="D6" t="s">
         <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>